<commit_message>
Update the floral morphology datasets
</commit_message>
<xml_diff>
--- a/Hemiboea_morph.xlsx
+++ b/Hemiboea_morph.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jing-yi.lu/Data-analysis-ecoevo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17DE74D-7F0A-B744-AB81-65D7D4179B75}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7C91EE-00E3-0446-9BD3-8013236D7B2A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{A31572D7-A256-E94E-AF35-D30157055603}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{A31572D7-A256-E94E-AF35-D30157055603}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Species</t>
   </si>
@@ -81,15 +81,9 @@
     <t>Hemiboea_wangiana</t>
   </si>
   <si>
-    <t>Lysionotus_chingii</t>
-  </si>
-  <si>
     <t>Briggsia_mihieri</t>
   </si>
   <si>
-    <t>Raphiocarpus_begoniifolius</t>
-  </si>
-  <si>
     <t>Capsule_length</t>
   </si>
   <si>
@@ -106,6 +100,9 @@
   </si>
   <si>
     <t>Pistill_length</t>
+  </si>
+  <si>
+    <t>Briggsia_longipes</t>
   </si>
 </sst>
 </file>
@@ -457,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5C0B0E-091B-9B4C-AF2B-056F90517E5A}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,22 +467,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" t="s">
-        <v>26</v>
-      </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -875,30 +872,30 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B19">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D19">
         <v>6</v>
       </c>
       <c r="E19">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F19">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G19">
-        <v>77.5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -917,29 +914,6 @@
       </c>
       <c r="G20">
         <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>22.5</v>
-      </c>
-      <c r="C21">
-        <v>45</v>
-      </c>
-      <c r="D21">
-        <v>6.5</v>
-      </c>
-      <c r="E21">
-        <v>14.5</v>
-      </c>
-      <c r="F21">
-        <v>34</v>
-      </c>
-      <c r="G21">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>